<commit_message>
Added an include to check for script directory Tweaked README.md Added a new command to the Excel file
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>attack</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Copy and paste above into smitten.ahk</t>
+  </si>
+  <si>
+    <t>way</t>
+  </si>
+  <si>
+    <t>VVVE</t>
   </si>
 </sst>
 </file>
@@ -738,9 +744,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -828,6 +831,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -883,16 +889,16 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D50" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="Column1" headerRowDxfId="1" dataDxfId="0">
+    <tableColumn id="1" name="Column1" headerRowDxfId="4" dataDxfId="3">
       <calculatedColumnFormula>IF(NOT(ISBLANK(dictionary!A2)),CONCATENATE("""",dictionary!A2,""""),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Column2" headerRowDxfId="2">
       <calculatedColumnFormula>IF(NOT(ISBLANK(dictionary!B2)),CONCATENATE("""",dictionary!B2,""""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Column3" headerRowDxfId="3">
+    <tableColumn id="3" name="Column3" headerRowDxfId="1">
       <calculatedColumnFormula>CONCATENATE($C1,",",$A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Column4" headerRowDxfId="4">
+    <tableColumn id="4" name="Column4" headerRowDxfId="0">
       <calculatedColumnFormula>CONCATENATE($D1,",",$B2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1187,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,7 +1216,7 @@
       </c>
       <c r="D1" t="str">
         <f>CONCATENATE("[",formulas!E1,"]")</f>
-        <v>["attack","behind","jungle","careful","defend","laugh","joke","missing","gank","help","incoming","ward","retreat","on it","buff","take","re","okay","b","mana","thanks","wait","cancel","nice","welcome","group","stay","trap","ultimate"]</v>
+        <v>["attack","behind","jungle","careful","defend","laugh","joke","missing","gank","help","incoming","ward","retreat","on it","buff","take","re","okay","b","mana","thanks","wait","cancel","nice","welcome","group","stay","trap","ultimate","way"]</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1222,7 +1228,7 @@
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("[",formulas!E2,"]")</f>
-        <v>["VAA","VVVB","VBJJ","VCC","VDD","VEL","VEJ","VFF","VGG","VHH","VII","VQN","VRR","VSO","VSBB","VSBT","VTT","VVA","VVB","VVM","VVT","VVW","VVX","VVGN","VVGW","VVVG","VVVS","VVVT","VVVR"]</v>
+        <v>["VAA","VVVB","VBJJ","VCC","VDD","VEL","VEJ","VFF","VGG","VHH","VII","VQN","VRR","VSO","VSBB","VSBT","VTT","VVA","VVB","VVM","VVT","VVW","VVX","VVGN","VVGW","VVVG","VVVS","VVVT","VVVR","VVVE"]</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,6 +1456,14 @@
       </c>
       <c r="B30" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1509,7 @@
       </c>
       <c r="E1" s="1" t="str">
         <f t="array" ref="E1">INDEX(formulas!C:C,MATCH(MAX(LEN(formulas!C:C)),LEN(formulas!C:C),0))</f>
-        <v>"attack","behind","jungle","careful","defend","laugh","joke","missing","gank","help","incoming","ward","retreat","on it","buff","take","re","okay","b","mana","thanks","wait","cancel","nice","welcome","group","stay","trap","ultimate"</v>
+        <v>"attack","behind","jungle","careful","defend","laugh","joke","missing","gank","help","incoming","ward","retreat","on it","buff","take","re","okay","b","mana","thanks","wait","cancel","nice","welcome","group","stay","trap","ultimate","way"</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1517,7 +1531,7 @@
       </c>
       <c r="E2" s="1" t="str">
         <f t="array" ref="E2">INDEX(formulas!D:D,MATCH(MAX(LEN(formulas!D:D)),LEN(formulas!D:D),0))</f>
-        <v>"VAA","VVVB","VBJJ","VCC","VDD","VEL","VEJ","VFF","VGG","VHH","VII","VQN","VRR","VSO","VSBB","VSBT","VTT","VVA","VVB","VVM","VVT","VVW","VVX","VVGN","VVGW","VVVG","VVVS","VVVT","VVVR"</v>
+        <v>"VAA","VVVB","VBJJ","VCC","VDD","VEL","VEJ","VFF","VGG","VHH","VII","VQN","VRR","VSO","VSBB","VSBT","VTT","VVA","VVB","VVM","VVT","VVW","VVX","VVGN","VVGW","VVVG","VVVS","VVVT","VVVR","VVVE"</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,19 +2023,19 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF(NOT(ISBLANK(dictionary!A31)),CONCATENATE("""",dictionary!A31,""""),"")</f>
-        <v/>
+        <v>"way"</v>
       </c>
       <c r="B30" t="str">
         <f>IF(NOT(ISBLANK(dictionary!B31)),CONCATENATE("""",dictionary!B31,""""),"")</f>
-        <v/>
+        <v>"VVVE"</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>"attack","behind","jungle","careful","defend","laugh","joke","missing","gank","help","incoming","ward","retreat","on it","buff","take","re","okay","b","mana","thanks","wait","cancel","nice","welcome","group","stay","trap","ultimate","way"</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>"VAA","VVVB","VBJJ","VCC","VDD","VEL","VEJ","VFF","VGG","VHH","VII","VQN","VRR","VSO","VSBB","VSBT","VTT","VVA","VVB","VVM","VVT","VVW","VVX","VVGN","VVGW","VVVG","VVVS","VVVT","VVVR","VVVE"</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>